<commit_message>
Everytime the code runs, a new excel file will be created.
</commit_message>
<xml_diff>
--- a/COTask.xlsx
+++ b/COTask.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GoSaas Labs\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GoSaas Labs\Documents\UiPath\COTask\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5770B46-0ABA-42E0-944F-4F81AFF7DA1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898B0B8B-642D-4EEB-A2CC-000B5A34F663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4785" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-4785" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Open" sheetId="2" r:id="rId2"/>
-    <sheet name="Approval" sheetId="3" r:id="rId3"/>
-    <sheet name="Scheduled" sheetId="6" r:id="rId4"/>
-    <sheet name="Completed" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -198,12 +198,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -218,13 +224,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,12 +588,12 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -863,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A91ECC33-7F29-4D7F-8A14-ED2D37115CCC}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1023,7 @@
       <c r="A8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C8" t="s">
@@ -1155,7 +1162,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,7 +1350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0FD729-0EA0-4198-87CE-16DD33113B21}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>

</xml_diff>